<commit_message>
[TECH] Removed password from the Excelsheet | Purushotham
</commit_message>
<xml_diff>
--- a/WandAutomation/ExcelFile/TimeSheetData.xlsx
+++ b/WandAutomation/ExcelFile/TimeSheetData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21713" windowHeight="8806"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21713" windowHeight="8806" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>purushv@thoughtworks.com</t>
   </si>
   <si>
-    <t>mckinsey@123</t>
-  </si>
-  <si>
     <t>BillingType</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>RegularHours</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -433,75 +433,75 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -539,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>